<commit_message>
Det function duikers revised
</commit_message>
<xml_diff>
--- a/data/duiker_vlm.xlsx
+++ b/data/duiker_vlm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\git\2D_DistanceSampling\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valentina.lamorgia/Documents/GitHub/2D_DistanceSampling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2DA341-4E5D-44E3-9A4A-B962BCF3FC99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D329ED-FECA-D64D-9FBE-51E69AD6616C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{20C80A23-CD56-47EA-B4F3-12F664F0BA5D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10300" xr2:uid="{20C80A23-CD56-47EA-B4F3-12F664F0BA5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="2" r:id="rId1"/>
@@ -287,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -309,7 +309,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -626,17 +625,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{969478A8-3B45-4784-A6E9-2DD3E3AA7CF0}">
   <dimension ref="A1:K83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="9" max="9" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -671,7 +670,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>487</v>
       </c>
@@ -706,7 +705,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>487</v>
       </c>
@@ -729,7 +728,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>487</v>
       </c>
@@ -752,7 +751,7 @@
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>487</v>
       </c>
@@ -787,7 +786,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>487</v>
       </c>
@@ -822,7 +821,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>487</v>
       </c>
@@ -857,7 +856,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>487</v>
       </c>
@@ -880,15 +879,15 @@
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>487</v>
       </c>
       <c r="B9" s="2">
         <v>7</v>
       </c>
-      <c r="C9" s="9">
-        <v>11829</v>
+      <c r="C9" s="3">
+        <v>11.829000000000001</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -903,7 +902,7 @@
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>487</v>
       </c>
@@ -926,7 +925,7 @@
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>487</v>
       </c>
@@ -949,7 +948,7 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>487</v>
       </c>
@@ -972,7 +971,7 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>487</v>
       </c>
@@ -995,7 +994,7 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>487</v>
       </c>
@@ -1018,7 +1017,7 @@
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>487</v>
       </c>
@@ -1041,7 +1040,7 @@
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>487</v>
       </c>
@@ -1064,7 +1063,7 @@
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>487</v>
       </c>
@@ -1099,7 +1098,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>487</v>
       </c>
@@ -1122,7 +1121,7 @@
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>487</v>
       </c>
@@ -1146,7 +1145,7 @@
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>487</v>
       </c>
@@ -1169,7 +1168,7 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>487</v>
       </c>
@@ -1193,7 +1192,7 @@
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>487</v>
       </c>
@@ -1216,7 +1215,7 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>487</v>
       </c>
@@ -1251,7 +1250,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>487</v>
       </c>
@@ -1274,7 +1273,7 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>487</v>
       </c>
@@ -1297,7 +1296,7 @@
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>487</v>
       </c>
@@ -1320,7 +1319,7 @@
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>487</v>
       </c>
@@ -1343,7 +1342,7 @@
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>487</v>
       </c>
@@ -1366,7 +1365,7 @@
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>487</v>
       </c>
@@ -1389,7 +1388,7 @@
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>487</v>
       </c>
@@ -1412,7 +1411,7 @@
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>487</v>
       </c>
@@ -1435,7 +1434,7 @@
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>487</v>
       </c>
@@ -1458,7 +1457,7 @@
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>487</v>
       </c>
@@ -1481,7 +1480,7 @@
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>487</v>
       </c>
@@ -1512,7 +1511,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>487</v>
       </c>
@@ -1535,7 +1534,7 @@
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>487</v>
       </c>
@@ -1570,7 +1569,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>487</v>
       </c>
@@ -1605,7 +1604,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>487</v>
       </c>
@@ -1640,7 +1639,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>487</v>
       </c>
@@ -1675,7 +1674,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>487</v>
       </c>
@@ -1710,7 +1709,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>487</v>
       </c>
@@ -1745,7 +1744,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>487</v>
       </c>
@@ -1780,7 +1779,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>487</v>
       </c>
@@ -1815,7 +1814,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>487</v>
       </c>
@@ -1850,7 +1849,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>487</v>
       </c>
@@ -1873,7 +1872,7 @@
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>487</v>
       </c>
@@ -1908,7 +1907,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>487</v>
       </c>
@@ -1931,7 +1930,7 @@
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>487</v>
       </c>
@@ -1966,7 +1965,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>487</v>
       </c>
@@ -2001,7 +2000,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>487</v>
       </c>
@@ -2024,7 +2023,7 @@
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>487</v>
       </c>
@@ -2047,7 +2046,7 @@
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>487</v>
       </c>
@@ -2070,7 +2069,7 @@
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>487</v>
       </c>
@@ -2093,7 +2092,7 @@
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>487</v>
       </c>
@@ -2116,7 +2115,7 @@
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>487</v>
       </c>
@@ -2139,7 +2138,7 @@
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>487</v>
       </c>
@@ -2162,7 +2161,7 @@
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>487</v>
       </c>
@@ -2197,7 +2196,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>487</v>
       </c>
@@ -2232,7 +2231,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>487</v>
       </c>
@@ -2255,7 +2254,7 @@
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>487</v>
       </c>
@@ -2278,7 +2277,7 @@
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>487</v>
       </c>
@@ -2301,7 +2300,7 @@
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>487</v>
       </c>
@@ -2324,7 +2323,7 @@
       <c r="J62" s="3"/>
       <c r="K62" s="3"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>487</v>
       </c>
@@ -2347,7 +2346,7 @@
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>487</v>
       </c>
@@ -2370,7 +2369,7 @@
       <c r="J64" s="3"/>
       <c r="K64" s="3"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>487</v>
       </c>
@@ -2393,7 +2392,7 @@
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>487</v>
       </c>
@@ -2416,7 +2415,7 @@
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>487</v>
       </c>
@@ -2439,7 +2438,7 @@
       <c r="J67" s="3"/>
       <c r="K67" s="3"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>487</v>
       </c>
@@ -2462,7 +2461,7 @@
       <c r="J68" s="3"/>
       <c r="K68" s="3"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>487</v>
       </c>
@@ -2497,7 +2496,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>487</v>
       </c>
@@ -2520,7 +2519,7 @@
       <c r="J70" s="3"/>
       <c r="K70" s="3"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>487</v>
       </c>
@@ -2543,7 +2542,7 @@
       <c r="J71" s="3"/>
       <c r="K71" s="3"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>487</v>
       </c>
@@ -2566,7 +2565,7 @@
       <c r="J72" s="3"/>
       <c r="K72" s="3"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>487</v>
       </c>
@@ -2601,7 +2600,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>487</v>
       </c>
@@ -2636,7 +2635,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>487</v>
       </c>
@@ -2659,7 +2658,7 @@
       <c r="J75" s="3"/>
       <c r="K75" s="3"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>487</v>
       </c>
@@ -2694,7 +2693,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>487</v>
       </c>
@@ -2729,7 +2728,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>487</v>
       </c>
@@ -2764,7 +2763,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>487</v>
       </c>
@@ -2799,7 +2798,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>487</v>
       </c>
@@ -2822,7 +2821,7 @@
       <c r="J80" s="3"/>
       <c r="K80" s="3"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>487</v>
       </c>
@@ -2845,7 +2844,7 @@
       <c r="J81" s="3"/>
       <c r="K81" s="3"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>487</v>
       </c>
@@ -2868,7 +2867,7 @@
       <c r="J82" s="3"/>
       <c r="K82" s="3"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>487</v>
       </c>

</xml_diff>